<commit_message>
models folder all updated, controller/auth/index.js and controller/index.js,resentation and excel updated
</commit_message>
<xml_diff>
--- a/assets/Book1.xlsx
+++ b/assets/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozdal\Gamersheim-Interactive-Full-Stack-Project-\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7CE91E-1C67-4CE6-AFBD-04E575AD20D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B7DD50-2EE1-4174-BF5D-6F64B41DCB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="639" firstSheet="3" activeTab="11" xr2:uid="{FAF77945-09F6-4FCB-A16D-3A474B64AE39}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="196">
   <si>
     <t>Genre Id</t>
   </si>
@@ -461,878 +461,13 @@
     <t>seed code</t>
   </si>
   <si>
-    <r>
-      <t>const</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> { </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4FC1FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>DataTypes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> } </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>require</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'sequelize'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>const</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>sequelize</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>require</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'../config/connection'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>);</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Game</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>extends</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Game</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>init</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-  </si>
-  <si>
     <t>  {</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>id:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>DataTypes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>INTEGER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>allowNull:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>false</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>primaryKey:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>autoIncrement:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
   </si>
   <si>
     <t>    },</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>title:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>DataTypes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>STRING</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>genre:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>publisher:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>platform:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>release_Year:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
     <t>  },</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>sequelize</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>timestamps:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>false</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>freezeTableName:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>underscored:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>modelName:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'games'</t>
-    </r>
   </si>
   <si>
     <t>  }</t>
@@ -1341,1349 +476,170 @@
     <t>);</t>
   </si>
   <si>
-    <r>
-      <t>module</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>exports</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Game</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Genre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>extends</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Genre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>init</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>genre_name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>modelName:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'genre'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>module</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>exports</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Genre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Platform</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>extends</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Platform</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>init</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>platform_name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>modelName:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'platform'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>module</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>exports</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Platform</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Userslibrary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>extends</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Userslibrary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>init</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>user_id:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>game_id:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>platform_id:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>played:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>DataTypes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>BOOLEAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>modelName:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'users_library'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>module</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>exports</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Userslibrary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Users</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>extends</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Users</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>init</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>user_name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>firs_name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>last_name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>email:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>unique:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>validate:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>isEmail:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF569CD6"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
     <t>      },</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>password:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {</t>
-    </r>
+    <t>const { Model, DataTypes } = require('sequelize');</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>len:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> [</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFB5CEA8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>],</t>
-    </r>
+    <t>const sequelize = require('../config/connection');</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>modelName:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>'user'</t>
-    </r>
+    <t>class Game extends Model {}</t>
   </si>
   <si>
-    <r>
-      <t>module</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>exports</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Users</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
+    <t>class Genre extends Model {}</t>
+  </si>
+  <si>
+    <t>class Platform extends Model {}</t>
+  </si>
+  <si>
+    <t>class Userslibrary extends Model {}</t>
+  </si>
+  <si>
+    <t>class Users extends Model {}</t>
+  </si>
+  <si>
+    <t>Game.init(</t>
+  </si>
+  <si>
+    <t>Genre.init(</t>
+  </si>
+  <si>
+    <t>Platform.init(</t>
+  </si>
+  <si>
+    <t>Userslibrary.init(</t>
+  </si>
+  <si>
+    <t>Users.init(</t>
+  </si>
+  <si>
+    <t>    id: {</t>
+  </si>
+  <si>
+    <t>      type: DataTypes.INTEGER,</t>
+  </si>
+  <si>
+    <t>      allowNull: false,</t>
+  </si>
+  <si>
+    <t>      primaryKey: true,</t>
+  </si>
+  <si>
+    <t>      autoIncrement: true,</t>
+  </si>
+  <si>
+    <t>    title: {</t>
+  </si>
+  <si>
+    <t>    genre_name: {</t>
+  </si>
+  <si>
+    <t>    platform_name: {</t>
+  </si>
+  <si>
+    <t>    user_id: {</t>
+  </si>
+  <si>
+    <t>    user_name: {</t>
+  </si>
+  <si>
+    <t>      type: DataTypes.STRING,</t>
+  </si>
+  <si>
+    <t>    sequelize,</t>
+  </si>
+  <si>
+    <t>    game_id: {</t>
+  </si>
+  <si>
+    <t>    firs_name: {</t>
+  </si>
+  <si>
+    <t>    timestamps: false,</t>
+  </si>
+  <si>
+    <t>    publisher: {</t>
+  </si>
+  <si>
+    <t>    freezeTableName: true,</t>
+  </si>
+  <si>
+    <t>    underscored: true,</t>
+  </si>
+  <si>
+    <t>    modelName: 'genre'</t>
+  </si>
+  <si>
+    <t>    modelName: 'platform'</t>
+  </si>
+  <si>
+    <t>    platform_id: {</t>
+  </si>
+  <si>
+    <t>    last_name: {</t>
+  </si>
+  <si>
+    <t>module.exports = Genre;</t>
+  </si>
+  <si>
+    <t>module.exports = Platform;</t>
+  </si>
+  <si>
+    <t>    release_Year: {</t>
+  </si>
+  <si>
+    <t>    played: {</t>
+  </si>
+  <si>
+    <t>    email: {</t>
+  </si>
+  <si>
+    <t>      type: DataTypes.BOOLEAN,</t>
+  </si>
+  <si>
+    <t>      unique: true,</t>
+  </si>
+  <si>
+    <t>      validate: {</t>
+  </si>
+  <si>
+    <t>        isEmail: true,</t>
+  </si>
+  <si>
+    <t>    modelName: 'games'</t>
+  </si>
+  <si>
+    <t>    password: {</t>
+  </si>
+  <si>
+    <t>    modelName: 'users_library'</t>
+  </si>
+  <si>
+    <t>module.exports = Game;</t>
+  </si>
+  <si>
+    <t>        len: [8],</t>
+  </si>
+  <si>
+    <t>module.exports = Userslibrary;</t>
+  </si>
+  <si>
+    <t>    modelName: 'user'</t>
+  </si>
+  <si>
+    <t>module.exports = Users;</t>
+  </si>
+  <si>
+    <t>    genre_id: {</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2727,60 +683,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF569CD6"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4EC9B0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4FC1FF"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFD4D4D4"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFDCDCAA"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFB5CEA8"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2797,7 +699,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1F1F1F"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2829,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2845,16 +747,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3352,707 +1249,717 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE2E20E-69BE-4238-AD02-CC4072115159}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I57"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="59.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="10"/>
+    <col min="5" max="5" width="59.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="10"/>
+    <col min="7" max="7" width="59.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="10"/>
+    <col min="9" max="9" width="59.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="A3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="E18" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="G4" s="9" t="s">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="E24" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="G27" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="I33" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="G40" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="G42" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="11"/>
+      <c r="I45" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G46" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I55" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="G27" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="I39" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="G42" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G44" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="I44" s="12" t="s">
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I57" s="9" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G45" s="10"/>
-      <c r="I45" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G46" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I47" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I48" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I49" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I50" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I51" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I52" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I53" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I54" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I55" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I56" s="10"/>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I57" s="11" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4294,7 +2201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BA949B-4B2A-4111-B1E1-4EE16CA82A73}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -4963,7 +2870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B261C1-4460-4C6E-8B62-203C29C91C43}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C57"/>
     </sheetView>
   </sheetViews>

</xml_diff>